<commit_message>
Add Transfer-Delta-T and Life-Support-Cost calculation.
Add Zero-Net-Income-Cost-Diff calculation.
</commit_message>
<xml_diff>
--- a/Interplanetary Transfer Sheet.xlsx
+++ b/Interplanetary Transfer Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="48">
   <si>
     <t>Sun</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -126,10 +126,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TransferWindow (earth day)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Isp(m/s)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -191,6 +187,34 @@
   </si>
   <si>
     <t>NetIncome ($)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TransferWindow (earth day^-1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TransferDeltaT (s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TransferDeltaT (earth day)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CrewCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LSCost ($)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LifeSupportCost ($/earth day)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZeroNetIncomeCostDiff ($/kg)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -533,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:J147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -812,6 +836,12 @@
         <v>4.5986176309124484E-8</v>
       </c>
     </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="str">
+        <f ca="1">INDIRECT("R"&amp;(ROW()+2)&amp;"C"&amp;COLUMN(),FALSE)</f>
+        <v>TransferWindow (s^-1)</v>
+      </c>
+    </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>24</v>
@@ -1215,7 +1245,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
         <v>15</v>
@@ -1616,7 +1646,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
@@ -2017,1302 +2047,2922 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>31</v>
-      </c>
-      <c r="B48">
-        <v>0.01</v>
+        <v>42</v>
+      </c>
+      <c r="B48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G48" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" t="s">
+        <v>20</v>
+      </c>
+      <c r="I48" t="s">
+        <v>21</v>
+      </c>
+      <c r="J48" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>32</v>
-      </c>
-      <c r="B49">
-        <v>5.0000000000000001E-3</v>
+        <v>15</v>
+      </c>
+      <c r="B49" s="1">
+        <f>PI() *SQRT(($C$3*$H$2+$C3*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>3800238.7346423175</v>
+      </c>
+      <c r="C49" s="1">
+        <f>PI() *SQRT(($C$4*$H$2+$C3*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>6527866.6654020986</v>
+      </c>
+      <c r="D49" s="1">
+        <f>PI() *SQRT(($C$5*$H$2+$C3*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>9113710.1833259389</v>
+      </c>
+      <c r="E49" s="1">
+        <f>PI() *SQRT(($C$6*$H$2+$C3*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>14734978.385472802</v>
+      </c>
+      <c r="F49" s="1">
+        <f>PI() *SQRT(($C$7*$H$2+$C3*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>73760993.283203334</v>
+      </c>
+      <c r="G49" s="1">
+        <f>PI() *SQRT(($C$8*$H$2+$C3*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>175613338.84389085</v>
+      </c>
+      <c r="H49" s="1">
+        <f>PI() *SQRT(($C$9*$H$2+$C3*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>484285329.38349134</v>
+      </c>
+      <c r="I49" s="1">
+        <f>PI() *SQRT(($C$10*$H$2+$C3*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>939555130.86022103</v>
+      </c>
+      <c r="J49" s="1">
+        <f>PI() *SQRT(($C$11*$H$2+$C3*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>1404288796.8002455</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="1">
+        <f t="shared" ref="B50:B57" si="30">PI() *SQRT(($C$3*$H$2+$C4*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>6527866.6654020986</v>
+      </c>
+      <c r="C50" s="1">
+        <f t="shared" ref="C50:C57" si="31">PI() *SQRT(($C$4*$H$2+$C4*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>9707021.8440248948</v>
+      </c>
+      <c r="D50" s="1">
+        <f t="shared" ref="D50:D57" si="32">PI() *SQRT(($C$5*$H$2+$C4*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>12620830.208783841</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" ref="E50:E57" si="33">PI() *SQRT(($C$6*$H$2+$C4*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>18790671.197622295</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" ref="F50:F57" si="34">PI() *SQRT(($C$7*$H$2+$C4*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>80513246.007939935</v>
+      </c>
+      <c r="G50" s="1">
+        <f t="shared" ref="G50:G57" si="35">PI() *SQRT(($C$8*$H$2+$C4*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>184571824.15825889</v>
+      </c>
+      <c r="H50" s="1">
+        <f t="shared" ref="H50:H56" si="36">PI() *SQRT(($C$9*$H$2+$C4*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>496796821.61977977</v>
+      </c>
+      <c r="I50" s="1">
+        <f t="shared" ref="I50:I57" si="37">PI() *SQRT(($C$10*$H$2+$C4*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>955135934.16256213</v>
+      </c>
+      <c r="J50" s="1">
+        <f t="shared" ref="J50:J57" si="38">PI() *SQRT(($C$11*$H$2+$C4*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>1422091589.9287226</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>33</v>
+        <v>2</v>
+      </c>
+      <c r="B51" s="1">
+        <f t="shared" si="30"/>
+        <v>9113710.1833259389</v>
+      </c>
+      <c r="C51" s="1">
+        <f t="shared" si="31"/>
+        <v>12620830.208783841</v>
+      </c>
+      <c r="D51" s="1">
+        <f t="shared" si="32"/>
+        <v>15779000.468076456</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="33"/>
+        <v>22365863.31144591</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="34"/>
+        <v>86215267.359916925</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" si="35"/>
+        <v>192053871.85980812</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="36"/>
+        <v>507171302.97188437</v>
+      </c>
+      <c r="I51" s="1">
+        <f t="shared" si="37"/>
+        <v>968020405.62204075</v>
+      </c>
+      <c r="J51" s="1">
+        <f t="shared" si="38"/>
+        <v>1436796466.6243665</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>3</v>
+      </c>
+      <c r="B52" s="1">
+        <f t="shared" si="30"/>
+        <v>14734978.385472802</v>
+      </c>
+      <c r="C52" s="1">
+        <f t="shared" si="31"/>
+        <v>18790671.197622295</v>
+      </c>
+      <c r="D52" s="1">
+        <f t="shared" si="32"/>
+        <v>22365863.31144591</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="33"/>
+        <v>29676980.544688888</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="34"/>
+        <v>97357882.351725116</v>
+      </c>
+      <c r="G52" s="1">
+        <f t="shared" si="35"/>
+        <v>206484456.20807004</v>
+      </c>
+      <c r="H52" s="1">
+        <f t="shared" si="36"/>
+        <v>527002798.70585692</v>
+      </c>
+      <c r="I52" s="1">
+        <f t="shared" si="37"/>
+        <v>992565213.94472587</v>
+      </c>
+      <c r="J52" s="1">
+        <f t="shared" si="38"/>
+        <v>1464767626.9547253</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>4</v>
+      </c>
+      <c r="B53" s="1">
+        <f t="shared" si="30"/>
+        <v>73760993.283203334</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" si="31"/>
+        <v>80513246.007939935</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" si="32"/>
+        <v>86215267.359916925</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="33"/>
+        <v>97357882.351725116</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="34"/>
+        <v>187342146.2557393</v>
+      </c>
+      <c r="G53" s="1">
+        <f t="shared" si="35"/>
+        <v>317215649.67149711</v>
+      </c>
+      <c r="H53" s="1">
+        <f t="shared" si="36"/>
+        <v>673329550.88545156</v>
+      </c>
+      <c r="I53" s="1">
+        <f t="shared" si="37"/>
+        <v>1170744815.8928881</v>
+      </c>
+      <c r="J53" s="1">
+        <f t="shared" si="38"/>
+        <v>1666358310.6250682</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>5</v>
+      </c>
+      <c r="B54" s="1">
+        <f t="shared" si="30"/>
+        <v>175613338.84389085</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" si="31"/>
+        <v>184571824.15825889</v>
+      </c>
+      <c r="D54" s="1">
+        <f t="shared" si="32"/>
+        <v>192053871.85980812</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="33"/>
+        <v>206484456.20807004</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="34"/>
+        <v>317215649.67149711</v>
+      </c>
+      <c r="G54" s="1">
+        <f t="shared" si="35"/>
+        <v>468063234.18971658</v>
+      </c>
+      <c r="H54" s="1">
+        <f t="shared" si="36"/>
+        <v>862275102.36256778</v>
+      </c>
+      <c r="I54" s="1">
+        <f t="shared" si="37"/>
+        <v>1395079050.0871747</v>
+      </c>
+      <c r="J54" s="1">
+        <f t="shared" si="38"/>
+        <v>1917168719.6577225</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="1">
+        <f t="shared" si="30"/>
+        <v>484285329.38349134</v>
+      </c>
+      <c r="C55" s="1">
+        <f t="shared" si="31"/>
+        <v>496796821.61977977</v>
+      </c>
+      <c r="D55" s="1">
+        <f t="shared" si="32"/>
+        <v>507171302.97188437</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="33"/>
+        <v>527002798.70585692</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="34"/>
+        <v>673329550.88545156</v>
+      </c>
+      <c r="G55" s="1">
+        <f t="shared" si="35"/>
+        <v>862275102.36256778</v>
+      </c>
+      <c r="H55" s="1">
+        <f t="shared" si="36"/>
+        <v>1329398950.171695</v>
+      </c>
+      <c r="I55" s="1">
+        <f t="shared" si="37"/>
+        <v>1932769391.032171</v>
+      </c>
+      <c r="J55" s="1">
+        <f t="shared" si="38"/>
+        <v>2508845345.8548551</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>7</v>
+      </c>
+      <c r="B56" s="1">
+        <f t="shared" si="30"/>
+        <v>939555130.86022103</v>
+      </c>
+      <c r="C56" s="1">
+        <f t="shared" si="31"/>
+        <v>955135934.16256213</v>
+      </c>
+      <c r="D56" s="1">
+        <f t="shared" si="32"/>
+        <v>968020405.62204075</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="33"/>
+        <v>992565213.94472587</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="34"/>
+        <v>1170744815.8928881</v>
+      </c>
+      <c r="G56" s="1">
+        <f t="shared" si="35"/>
+        <v>1395079050.0871747</v>
+      </c>
+      <c r="H56" s="1">
+        <f t="shared" si="36"/>
+        <v>1932769391.032171</v>
+      </c>
+      <c r="I56" s="1">
+        <f t="shared" si="37"/>
+        <v>2607027560.1113849</v>
+      </c>
+      <c r="J56" s="1">
+        <f t="shared" si="38"/>
+        <v>3238580900.4902244</v>
       </c>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57">
-        <v>7200</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
-      <c r="A58" t="s">
-        <v>27</v>
+      <c r="A57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="1">
+        <f t="shared" si="30"/>
+        <v>1404288796.8002455</v>
+      </c>
+      <c r="C57" s="1">
+        <f t="shared" si="31"/>
+        <v>1422091589.9287226</v>
+      </c>
+      <c r="D57" s="1">
+        <f t="shared" si="32"/>
+        <v>1436796466.6243665</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="33"/>
+        <v>1464767626.9547253</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="34"/>
+        <v>1666358310.6250682</v>
+      </c>
+      <c r="G57" s="1">
+        <f t="shared" si="35"/>
+        <v>1917168719.6577225</v>
+      </c>
+      <c r="H57" s="1">
+        <f>PI() *SQRT(($C$9*$H$2+$C11*$H$2)^3/8/$B$2/$G$2)</f>
+        <v>2508845345.8548551</v>
+      </c>
+      <c r="I57" s="1">
+        <f t="shared" si="37"/>
+        <v>3238580900.4902244</v>
+      </c>
+      <c r="J57" s="1">
+        <f t="shared" si="38"/>
+        <v>3914219760.0865712</v>
       </c>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59">
-        <v>50000</v>
+      <c r="A59" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" t="s">
+        <v>18</v>
+      </c>
+      <c r="F59" t="s">
+        <v>4</v>
+      </c>
+      <c r="G59" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" t="s">
+        <v>20</v>
+      </c>
+      <c r="I59" t="s">
+        <v>21</v>
+      </c>
+      <c r="J59" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="B60" s="2">
+        <f>B49/24/3600</f>
+        <v>43.984244613915706</v>
+      </c>
+      <c r="C60" s="2">
+        <f t="shared" ref="C60:J60" si="39">C49/24/3600</f>
+        <v>75.554012331042813</v>
+      </c>
+      <c r="D60" s="2">
+        <f t="shared" si="39"/>
+        <v>105.48275675145761</v>
+      </c>
+      <c r="E60" s="2">
+        <f t="shared" si="39"/>
+        <v>170.54373131334262</v>
+      </c>
+      <c r="F60" s="2">
+        <f t="shared" si="39"/>
+        <v>853.71520003707565</v>
+      </c>
+      <c r="G60" s="2">
+        <f t="shared" si="39"/>
+        <v>2032.5617921746625</v>
+      </c>
+      <c r="H60" s="2">
+        <f t="shared" si="39"/>
+        <v>5605.1542752718906</v>
+      </c>
+      <c r="I60" s="2">
+        <f t="shared" si="39"/>
+        <v>10874.480681252558</v>
+      </c>
+      <c r="J60" s="2">
+        <f t="shared" si="39"/>
+        <v>16253.342555558398</v>
       </c>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" t="e">
-        <f>A59*0.01+A63*0.03</f>
-        <v>#VALUE!</v>
+      <c r="A61" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" s="2">
+        <f t="shared" ref="B61:J61" si="40">B50/24/3600</f>
+        <v>75.554012331042813</v>
+      </c>
+      <c r="C61" s="2">
+        <f t="shared" si="40"/>
+        <v>112.34978986139924</v>
+      </c>
+      <c r="D61" s="2">
+        <f t="shared" si="40"/>
+        <v>146.07442371277594</v>
+      </c>
+      <c r="E61" s="2">
+        <f t="shared" si="40"/>
+        <v>217.48462034285066</v>
+      </c>
+      <c r="F61" s="2">
+        <f t="shared" si="40"/>
+        <v>931.86627324004553</v>
+      </c>
+      <c r="G61" s="2">
+        <f t="shared" si="40"/>
+        <v>2136.2479647946629</v>
+      </c>
+      <c r="H61" s="2">
+        <f t="shared" si="40"/>
+        <v>5749.9632131918952</v>
+      </c>
+      <c r="I61" s="2">
+        <f t="shared" si="40"/>
+        <v>11054.814052807433</v>
+      </c>
+      <c r="J61" s="2">
+        <f t="shared" si="40"/>
+        <v>16459.39340195281</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>29</v>
-      </c>
-      <c r="B62" t="s">
-        <v>15</v>
-      </c>
-      <c r="C62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D62" t="s">
-        <v>17</v>
-      </c>
-      <c r="E62" t="s">
-        <v>18</v>
-      </c>
-      <c r="F62" t="s">
-        <v>4</v>
-      </c>
-      <c r="G62" t="s">
-        <v>19</v>
-      </c>
-      <c r="H62" t="s">
-        <v>20</v>
-      </c>
-      <c r="I62" t="s">
-        <v>21</v>
-      </c>
-      <c r="J62" t="s">
-        <v>22</v>
+        <v>2</v>
+      </c>
+      <c r="B62" s="2">
+        <f t="shared" ref="B62:J62" si="41">B51/24/3600</f>
+        <v>105.48275675145761</v>
+      </c>
+      <c r="C62" s="2">
+        <f t="shared" si="41"/>
+        <v>146.07442371277594</v>
+      </c>
+      <c r="D62" s="2">
+        <f t="shared" si="41"/>
+        <v>182.6273202323664</v>
+      </c>
+      <c r="E62" s="2">
+        <f t="shared" si="41"/>
+        <v>258.86415869729063</v>
+      </c>
+      <c r="F62" s="2">
+        <f t="shared" si="41"/>
+        <v>997.86189073977926</v>
+      </c>
+      <c r="G62" s="2">
+        <f t="shared" si="41"/>
+        <v>2222.8457391181496</v>
+      </c>
+      <c r="H62" s="2">
+        <f t="shared" si="41"/>
+        <v>5870.0382288412538</v>
+      </c>
+      <c r="I62" s="2">
+        <f t="shared" si="41"/>
+        <v>11203.939879884731</v>
+      </c>
+      <c r="J62" s="2">
+        <f t="shared" si="41"/>
+        <v>16629.588734078316</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>15</v>
-      </c>
-      <c r="B63" t="e">
-        <f>$A$59 * (1+$B$48) / ( 1 / (EXP(B38 / $A$57) - 1) - $B$49)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C63">
-        <f t="shared" ref="C63:J63" si="30">$A$59 * (1+$B$48) / ( 1 / (EXP(C38 / $A$57) - 1) - $B$49)</f>
-        <v>243764.6281665932</v>
-      </c>
-      <c r="D63">
-        <f t="shared" si="30"/>
-        <v>521386.27569721697</v>
-      </c>
-      <c r="E63">
-        <f t="shared" si="30"/>
-        <v>1024057.582401467</v>
-      </c>
-      <c r="F63">
-        <f t="shared" si="30"/>
-        <v>2084145.1673505814</v>
-      </c>
-      <c r="G63">
-        <f t="shared" si="30"/>
-        <v>2013941.8647301318</v>
-      </c>
-      <c r="H63">
-        <f t="shared" si="30"/>
-        <v>1745781.1804861494</v>
-      </c>
-      <c r="I63">
-        <f t="shared" si="30"/>
-        <v>1568358.393027497</v>
-      </c>
-      <c r="J63">
-        <f t="shared" si="30"/>
-        <v>1472082.0106659322</v>
+        <v>3</v>
+      </c>
+      <c r="B63" s="2">
+        <f t="shared" ref="B63:J63" si="42">B52/24/3600</f>
+        <v>170.54373131334262</v>
+      </c>
+      <c r="C63" s="2">
+        <f t="shared" si="42"/>
+        <v>217.48462034285066</v>
+      </c>
+      <c r="D63" s="2">
+        <f t="shared" si="42"/>
+        <v>258.86415869729063</v>
+      </c>
+      <c r="E63" s="2">
+        <f t="shared" si="42"/>
+        <v>343.48357111908439</v>
+      </c>
+      <c r="F63" s="2">
+        <f t="shared" si="42"/>
+        <v>1126.8273420338555</v>
+      </c>
+      <c r="G63" s="2">
+        <f t="shared" si="42"/>
+        <v>2389.8663912971069</v>
+      </c>
+      <c r="H63" s="2">
+        <f t="shared" si="42"/>
+        <v>6099.569429465937</v>
+      </c>
+      <c r="I63" s="2">
+        <f t="shared" si="42"/>
+        <v>11488.023309545439</v>
+      </c>
+      <c r="J63" s="2">
+        <f t="shared" si="42"/>
+        <v>16953.32901567969</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>1</v>
-      </c>
-      <c r="B64">
-        <f t="shared" ref="B64:J71" si="31">$A$59 * (1+$B$48) / ( 1 / (EXP(B39 / $A$57) - 1) - $B$49)</f>
-        <v>243764.6281665932</v>
-      </c>
-      <c r="C64" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D64">
-        <f t="shared" si="31"/>
-        <v>53793.312183188784</v>
-      </c>
-      <c r="E64">
-        <f t="shared" si="31"/>
-        <v>170357.59335473482</v>
-      </c>
-      <c r="F64">
-        <f t="shared" si="31"/>
-        <v>597416.10874703818</v>
-      </c>
-      <c r="G64">
-        <f t="shared" si="31"/>
-        <v>674835.68927546986</v>
-      </c>
-      <c r="H64">
-        <f t="shared" si="31"/>
-        <v>654682.87329512485</v>
-      </c>
-      <c r="I64">
-        <f t="shared" si="31"/>
-        <v>615070.89962131891</v>
-      </c>
-      <c r="J64">
-        <f t="shared" si="31"/>
-        <v>588616.91867980035</v>
+        <v>4</v>
+      </c>
+      <c r="B64" s="2">
+        <f t="shared" ref="B64:J64" si="43">B53/24/3600</f>
+        <v>853.71520003707565</v>
+      </c>
+      <c r="C64" s="2">
+        <f t="shared" si="43"/>
+        <v>931.86627324004553</v>
+      </c>
+      <c r="D64" s="2">
+        <f t="shared" si="43"/>
+        <v>997.86189073977926</v>
+      </c>
+      <c r="E64" s="2">
+        <f t="shared" si="43"/>
+        <v>1126.8273420338555</v>
+      </c>
+      <c r="F64" s="2">
+        <f t="shared" si="43"/>
+        <v>2168.3118779599458</v>
+      </c>
+      <c r="G64" s="2">
+        <f t="shared" si="43"/>
+        <v>3671.477426753439</v>
+      </c>
+      <c r="H64" s="2">
+        <f t="shared" si="43"/>
+        <v>7793.1660982112453</v>
+      </c>
+      <c r="I64" s="2">
+        <f t="shared" si="43"/>
+        <v>13550.287220982502</v>
+      </c>
+      <c r="J64" s="2">
+        <f t="shared" si="43"/>
+        <v>19286.554521123471</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>2</v>
-      </c>
-      <c r="B65">
-        <f t="shared" si="31"/>
-        <v>521386.27569721697</v>
-      </c>
-      <c r="C65">
-        <f t="shared" si="31"/>
-        <v>53793.312183188784</v>
-      </c>
-      <c r="D65" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E65">
-        <f t="shared" si="31"/>
-        <v>59672.928708066633</v>
-      </c>
-      <c r="F65">
-        <f t="shared" si="31"/>
-        <v>335347.94887403568</v>
-      </c>
-      <c r="G65">
-        <f t="shared" si="31"/>
-        <v>415159.49602988188</v>
-      </c>
-      <c r="H65">
-        <f t="shared" si="31"/>
-        <v>429107.42947451596</v>
-      </c>
-      <c r="I65">
-        <f t="shared" si="31"/>
-        <v>413125.55568770255</v>
-      </c>
-      <c r="J65">
-        <f t="shared" si="31"/>
-        <v>399464.36888416781</v>
+        <v>5</v>
+      </c>
+      <c r="B65" s="2">
+        <f t="shared" ref="B65:J65" si="44">B54/24/3600</f>
+        <v>2032.5617921746625</v>
+      </c>
+      <c r="C65" s="2">
+        <f t="shared" si="44"/>
+        <v>2136.2479647946629</v>
+      </c>
+      <c r="D65" s="2">
+        <f t="shared" si="44"/>
+        <v>2222.8457391181496</v>
+      </c>
+      <c r="E65" s="2">
+        <f t="shared" si="44"/>
+        <v>2389.8663912971069</v>
+      </c>
+      <c r="F65" s="2">
+        <f t="shared" si="44"/>
+        <v>3671.477426753439</v>
+      </c>
+      <c r="G65" s="2">
+        <f t="shared" si="44"/>
+        <v>5417.3985438624604</v>
+      </c>
+      <c r="H65" s="2">
+        <f t="shared" si="44"/>
+        <v>9980.0359069741644</v>
+      </c>
+      <c r="I65" s="2">
+        <f t="shared" si="44"/>
+        <v>16146.748264897855</v>
+      </c>
+      <c r="J65" s="2">
+        <f t="shared" si="44"/>
+        <v>22189.452773816232</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>3</v>
-      </c>
-      <c r="B66">
-        <f t="shared" si="31"/>
-        <v>1024057.582401467</v>
-      </c>
-      <c r="C66">
-        <f t="shared" si="31"/>
-        <v>170357.59335473482</v>
-      </c>
-      <c r="D66">
-        <f t="shared" si="31"/>
-        <v>59672.928708066633</v>
-      </c>
-      <c r="E66" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F66">
-        <f t="shared" si="31"/>
-        <v>158814.87993556799</v>
-      </c>
-      <c r="G66">
-        <f t="shared" si="31"/>
-        <v>227490.18555083894</v>
-      </c>
-      <c r="H66">
-        <f t="shared" si="31"/>
-        <v>259277.49620016522</v>
-      </c>
-      <c r="I66">
-        <f t="shared" si="31"/>
-        <v>259215.26963789956</v>
-      </c>
-      <c r="J66">
-        <f t="shared" si="31"/>
-        <v>254672.52174875044</v>
+        <v>6</v>
+      </c>
+      <c r="B66" s="2">
+        <f t="shared" ref="B66:J66" si="45">B55/24/3600</f>
+        <v>5605.1542752718906</v>
+      </c>
+      <c r="C66" s="2">
+        <f t="shared" si="45"/>
+        <v>5749.9632131918952</v>
+      </c>
+      <c r="D66" s="2">
+        <f t="shared" si="45"/>
+        <v>5870.0382288412538</v>
+      </c>
+      <c r="E66" s="2">
+        <f t="shared" si="45"/>
+        <v>6099.569429465937</v>
+      </c>
+      <c r="F66" s="2">
+        <f t="shared" si="45"/>
+        <v>7793.1660982112453</v>
+      </c>
+      <c r="G66" s="2">
+        <f t="shared" si="45"/>
+        <v>9980.0359069741644</v>
+      </c>
+      <c r="H66" s="2">
+        <f t="shared" si="45"/>
+        <v>15386.561923283507</v>
+      </c>
+      <c r="I66" s="2">
+        <f t="shared" si="45"/>
+        <v>22370.016099909386</v>
+      </c>
+      <c r="J66" s="2">
+        <f t="shared" si="45"/>
+        <v>29037.561873320079</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>4</v>
-      </c>
-      <c r="B67">
-        <f t="shared" si="31"/>
-        <v>2084145.1673505814</v>
-      </c>
-      <c r="C67">
-        <f t="shared" si="31"/>
-        <v>597416.10874703818</v>
-      </c>
-      <c r="D67">
-        <f t="shared" si="31"/>
-        <v>335347.94887403568</v>
-      </c>
-      <c r="E67">
-        <f t="shared" si="31"/>
-        <v>158814.87993556799</v>
-      </c>
-      <c r="F67" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G67">
-        <f t="shared" si="31"/>
-        <v>30084.711640189969</v>
-      </c>
-      <c r="H67">
-        <f t="shared" si="31"/>
-        <v>61040.298692397591</v>
-      </c>
-      <c r="I67">
-        <f t="shared" si="31"/>
-        <v>74152.75883717493</v>
-      </c>
-      <c r="J67">
-        <f t="shared" si="31"/>
-        <v>79105.095118123631</v>
+        <v>7</v>
+      </c>
+      <c r="B67" s="2">
+        <f t="shared" ref="B67:J67" si="46">B56/24/3600</f>
+        <v>10874.480681252558</v>
+      </c>
+      <c r="C67" s="2">
+        <f t="shared" si="46"/>
+        <v>11054.814052807433</v>
+      </c>
+      <c r="D67" s="2">
+        <f t="shared" si="46"/>
+        <v>11203.939879884731</v>
+      </c>
+      <c r="E67" s="2">
+        <f t="shared" si="46"/>
+        <v>11488.023309545439</v>
+      </c>
+      <c r="F67" s="2">
+        <f t="shared" si="46"/>
+        <v>13550.287220982502</v>
+      </c>
+      <c r="G67" s="2">
+        <f t="shared" si="46"/>
+        <v>16146.748264897855</v>
+      </c>
+      <c r="H67" s="2">
+        <f t="shared" si="46"/>
+        <v>22370.016099909386</v>
+      </c>
+      <c r="I67" s="2">
+        <f t="shared" si="46"/>
+        <v>30173.930093881769</v>
+      </c>
+      <c r="J67" s="2">
+        <f t="shared" si="46"/>
+        <v>37483.575237155375</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>5</v>
-      </c>
-      <c r="B68">
-        <f t="shared" si="31"/>
-        <v>2013941.8647301318</v>
-      </c>
-      <c r="C68">
-        <f t="shared" si="31"/>
-        <v>674835.68927546986</v>
-      </c>
-      <c r="D68">
-        <f t="shared" si="31"/>
-        <v>415159.49602988188</v>
-      </c>
-      <c r="E68">
-        <f t="shared" si="31"/>
-        <v>227490.18555083894</v>
-      </c>
-      <c r="F68">
-        <f t="shared" si="31"/>
-        <v>30084.711640189969</v>
-      </c>
-      <c r="G68" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H68">
-        <f t="shared" si="31"/>
-        <v>23497.420251868662</v>
-      </c>
-      <c r="I68">
-        <f t="shared" si="31"/>
-        <v>36262.962197345376</v>
-      </c>
-      <c r="J68">
-        <f t="shared" si="31"/>
-        <v>42232.629672055038</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
-      <c r="A69" t="s">
-        <v>6</v>
-      </c>
-      <c r="B69">
-        <f t="shared" si="31"/>
-        <v>1745781.1804861494</v>
-      </c>
-      <c r="C69">
-        <f t="shared" si="31"/>
-        <v>654682.87329512485</v>
-      </c>
-      <c r="D69">
-        <f t="shared" si="31"/>
-        <v>429107.42947451596</v>
-      </c>
-      <c r="E69">
-        <f t="shared" si="31"/>
-        <v>259277.49620016522</v>
-      </c>
-      <c r="F69">
-        <f t="shared" si="31"/>
-        <v>61040.298692397591</v>
-      </c>
-      <c r="G69">
-        <f t="shared" si="31"/>
-        <v>23497.420251868662</v>
-      </c>
-      <c r="H69" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I69">
-        <f t="shared" si="31"/>
-        <v>10419.135403255701</v>
-      </c>
-      <c r="J69">
-        <f t="shared" si="31"/>
-        <v>16105.199648209251</v>
+        <v>13</v>
+      </c>
+      <c r="B68" s="2">
+        <f t="shared" ref="B68:J68" si="47">B57/24/3600</f>
+        <v>16253.342555558398</v>
+      </c>
+      <c r="C68" s="2">
+        <f t="shared" si="47"/>
+        <v>16459.39340195281</v>
+      </c>
+      <c r="D68" s="2">
+        <f t="shared" si="47"/>
+        <v>16629.588734078316</v>
+      </c>
+      <c r="E68" s="2">
+        <f t="shared" si="47"/>
+        <v>16953.32901567969</v>
+      </c>
+      <c r="F68" s="2">
+        <f t="shared" si="47"/>
+        <v>19286.554521123471</v>
+      </c>
+      <c r="G68" s="2">
+        <f t="shared" si="47"/>
+        <v>22189.452773816232</v>
+      </c>
+      <c r="H68" s="2">
+        <f t="shared" si="47"/>
+        <v>29037.561873320079</v>
+      </c>
+      <c r="I68" s="2">
+        <f t="shared" si="47"/>
+        <v>37483.575237155375</v>
+      </c>
+      <c r="J68" s="2">
+        <f t="shared" si="47"/>
+        <v>45303.469445446426</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B70">
-        <f t="shared" si="31"/>
-        <v>1568358.393027497</v>
-      </c>
-      <c r="C70">
-        <f t="shared" si="31"/>
-        <v>615070.89962131891</v>
-      </c>
-      <c r="D70">
-        <f t="shared" si="31"/>
-        <v>413125.55568770255</v>
-      </c>
-      <c r="E70">
-        <f t="shared" si="31"/>
-        <v>259215.26963789956</v>
-      </c>
-      <c r="F70">
-        <f t="shared" si="31"/>
-        <v>74152.75883717493</v>
-      </c>
-      <c r="G70">
-        <f t="shared" si="31"/>
-        <v>36262.962197345376</v>
-      </c>
-      <c r="H70">
-        <f t="shared" si="31"/>
-        <v>10419.135403255701</v>
-      </c>
-      <c r="I70" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J70">
-        <f t="shared" si="31"/>
-        <v>5039.5840465942847</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B71">
-        <f t="shared" si="31"/>
-        <v>1472082.0106659322</v>
-      </c>
-      <c r="C71">
-        <f t="shared" si="31"/>
-        <v>588616.91867980035</v>
-      </c>
-      <c r="D71">
-        <f t="shared" si="31"/>
-        <v>399464.36888416781</v>
-      </c>
-      <c r="E71">
-        <f t="shared" si="31"/>
-        <v>254672.52174875044</v>
-      </c>
-      <c r="F71">
-        <f t="shared" si="31"/>
-        <v>79105.095118123631</v>
-      </c>
-      <c r="G71">
-        <f t="shared" si="31"/>
-        <v>42232.629672055038</v>
-      </c>
-      <c r="H71">
-        <f t="shared" si="31"/>
-        <v>16105.199648209251</v>
-      </c>
-      <c r="I71">
-        <f t="shared" si="31"/>
-        <v>5039.5840465942847</v>
-      </c>
-      <c r="J71" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="B73">
+        <v>0.01</v>
       </c>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" t="s">
-        <v>38</v>
+      <c r="A74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74">
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76">
-        <f>A74*A59</f>
-        <v>750000</v>
+      <c r="A76" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
-      <c r="A80" t="s">
-        <v>40</v>
-      </c>
-      <c r="B80" t="s">
-        <v>15</v>
-      </c>
-      <c r="C80" t="s">
-        <v>16</v>
-      </c>
-      <c r="D80" t="s">
-        <v>17</v>
-      </c>
-      <c r="E80" t="s">
-        <v>18</v>
-      </c>
-      <c r="F80" t="s">
-        <v>4</v>
-      </c>
-      <c r="G80" t="s">
-        <v>19</v>
-      </c>
-      <c r="H80" t="s">
-        <v>20</v>
-      </c>
-      <c r="I80" t="s">
-        <v>21</v>
-      </c>
-      <c r="J80" t="s">
-        <v>22</v>
+      <c r="A78" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>15</v>
-      </c>
-      <c r="B81" t="e">
-        <f>B63*$A$78</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C81">
-        <f>C63*$A$78</f>
-        <v>731293.88449977967</v>
-      </c>
-      <c r="D81">
-        <f>D63*$A$78</f>
-        <v>1564158.827091651</v>
-      </c>
-      <c r="E81">
-        <f>E63*$A$78</f>
-        <v>3072172.7472044011</v>
-      </c>
-      <c r="F81">
-        <f>F63*$A$78</f>
-        <v>6252435.5020517446</v>
-      </c>
-      <c r="G81">
-        <f>G63*$A$78</f>
-        <v>6041825.5941903954</v>
-      </c>
-      <c r="H81">
-        <f>H63*$A$78</f>
-        <v>5237343.5414584484</v>
-      </c>
-      <c r="I81">
-        <f>I63*$A$78</f>
-        <v>4705075.1790824905</v>
-      </c>
-      <c r="J81">
-        <f>J63*$A$78</f>
-        <v>4416246.0319977961</v>
+        <v>25</v>
       </c>
     </row>
     <row r="82" spans="1:10">
-      <c r="A82" t="s">
-        <v>1</v>
-      </c>
-      <c r="B82">
-        <f>B64*$A$78</f>
-        <v>731293.88449977967</v>
-      </c>
-      <c r="C82" t="e">
-        <f>C64*$A$78</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D82">
-        <f>D64*$A$78</f>
-        <v>161379.93654956634</v>
-      </c>
-      <c r="E82">
-        <f>E64*$A$78</f>
-        <v>511072.78006420447</v>
-      </c>
-      <c r="F82">
-        <f>F64*$A$78</f>
-        <v>1792248.3262411146</v>
-      </c>
-      <c r="G82">
-        <f>G64*$A$78</f>
-        <v>2024507.0678264096</v>
-      </c>
-      <c r="H82">
-        <f>H64*$A$78</f>
-        <v>1964048.6198853746</v>
-      </c>
-      <c r="I82">
-        <f>I64*$A$78</f>
-        <v>1845212.6988639566</v>
-      </c>
-      <c r="J82">
-        <f>J64*$A$78</f>
-        <v>1765850.7560394011</v>
+      <c r="A82">
+        <v>7200</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>2</v>
-      </c>
-      <c r="B83">
-        <f>B65*$A$78</f>
-        <v>1564158.827091651</v>
-      </c>
-      <c r="C83">
-        <f>C65*$A$78</f>
-        <v>161379.93654956634</v>
-      </c>
-      <c r="D83" t="e">
-        <f>D65*$A$78</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E83">
-        <f>E65*$A$78</f>
-        <v>179018.78612419989</v>
-      </c>
-      <c r="F83">
-        <f>F65*$A$78</f>
-        <v>1006043.8466221071</v>
-      </c>
-      <c r="G83">
-        <f>G65*$A$78</f>
-        <v>1245478.4880896457</v>
-      </c>
-      <c r="H83">
-        <f>H65*$A$78</f>
-        <v>1287322.288423548</v>
-      </c>
-      <c r="I83">
-        <f>I65*$A$78</f>
-        <v>1239376.6670631077</v>
-      </c>
-      <c r="J83">
-        <f>J65*$A$78</f>
-        <v>1198393.1066525034</v>
+        <v>26</v>
       </c>
     </row>
     <row r="84" spans="1:10">
-      <c r="A84" t="s">
-        <v>3</v>
-      </c>
-      <c r="B84">
-        <f>B66*$A$78</f>
-        <v>3072172.7472044011</v>
-      </c>
-      <c r="C84">
-        <f>C66*$A$78</f>
-        <v>511072.78006420447</v>
-      </c>
-      <c r="D84">
-        <f>D66*$A$78</f>
-        <v>179018.78612419989</v>
-      </c>
-      <c r="E84" t="e">
-        <f>E66*$A$78</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F84">
-        <f>F66*$A$78</f>
-        <v>476444.63980670401</v>
-      </c>
-      <c r="G84">
-        <f>G66*$A$78</f>
-        <v>682470.55665251683</v>
-      </c>
-      <c r="H84">
-        <f>H66*$A$78</f>
-        <v>777832.48860049562</v>
-      </c>
-      <c r="I84">
-        <f>I66*$A$78</f>
-        <v>777645.80891369865</v>
-      </c>
-      <c r="J84">
-        <f>J66*$A$78</f>
-        <v>764017.5652462513</v>
+      <c r="A84">
+        <v>50000</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>4</v>
-      </c>
-      <c r="B85">
-        <f>B67*$A$78</f>
-        <v>6252435.5020517446</v>
-      </c>
-      <c r="C85">
-        <f>C67*$A$78</f>
-        <v>1792248.3262411146</v>
-      </c>
-      <c r="D85">
-        <f>D67*$A$78</f>
-        <v>1006043.8466221071</v>
-      </c>
-      <c r="E85">
-        <f>E67*$A$78</f>
-        <v>476444.63980670401</v>
-      </c>
-      <c r="F85" t="e">
-        <f>F67*$A$78</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G85">
-        <f>G67*$A$78</f>
-        <v>90254.134920569908</v>
-      </c>
-      <c r="H85">
-        <f>H67*$A$78</f>
-        <v>183120.89607719277</v>
-      </c>
-      <c r="I85">
-        <f>I67*$A$78</f>
-        <v>222458.2765115248</v>
-      </c>
-      <c r="J85">
-        <f>J67*$A$78</f>
-        <v>237315.28535437089</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86" spans="1:10">
-      <c r="A86" t="s">
-        <v>5</v>
-      </c>
-      <c r="B86">
-        <f>B68*$A$78</f>
-        <v>6041825.5941903954</v>
-      </c>
-      <c r="C86">
-        <f>C68*$A$78</f>
-        <v>2024507.0678264096</v>
-      </c>
-      <c r="D86">
-        <f>D68*$A$78</f>
-        <v>1245478.4880896457</v>
-      </c>
-      <c r="E86">
-        <f>E68*$A$78</f>
-        <v>682470.55665251683</v>
-      </c>
-      <c r="F86">
-        <f>F68*$A$78</f>
-        <v>90254.134920569908</v>
-      </c>
-      <c r="G86" t="e">
-        <f>G68*$A$78</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H86">
-        <f>H68*$A$78</f>
-        <v>70492.260755605981</v>
-      </c>
-      <c r="I86">
-        <f>I68*$A$78</f>
-        <v>108788.88659203613</v>
-      </c>
-      <c r="J86">
-        <f>J68*$A$78</f>
-        <v>126697.88901616511</v>
+      <c r="A86" t="e">
+        <f>A84*0.01+A88*0.03</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>6</v>
-      </c>
-      <c r="B87">
-        <f>B69*$A$78</f>
-        <v>5237343.5414584484</v>
-      </c>
-      <c r="C87">
-        <f>C69*$A$78</f>
-        <v>1964048.6198853746</v>
-      </c>
-      <c r="D87">
-        <f>D69*$A$78</f>
-        <v>1287322.288423548</v>
-      </c>
-      <c r="E87">
-        <f>E69*$A$78</f>
-        <v>777832.48860049562</v>
-      </c>
-      <c r="F87">
-        <f>F69*$A$78</f>
-        <v>183120.89607719277</v>
-      </c>
-      <c r="G87">
-        <f>G69*$A$78</f>
-        <v>70492.260755605981</v>
-      </c>
-      <c r="H87" t="e">
-        <f>H69*$A$78</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I87">
-        <f>I69*$A$78</f>
-        <v>31257.406209767105</v>
-      </c>
-      <c r="J87">
-        <f>J69*$A$78</f>
-        <v>48315.598944627753</v>
+        <v>28</v>
+      </c>
+      <c r="B87" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" t="s">
+        <v>16</v>
+      </c>
+      <c r="D87" t="s">
+        <v>17</v>
+      </c>
+      <c r="E87" t="s">
+        <v>18</v>
+      </c>
+      <c r="F87" t="s">
+        <v>4</v>
+      </c>
+      <c r="G87" t="s">
+        <v>19</v>
+      </c>
+      <c r="H87" t="s">
+        <v>20</v>
+      </c>
+      <c r="I87" t="s">
+        <v>21</v>
+      </c>
+      <c r="J87" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>7</v>
-      </c>
-      <c r="B88">
-        <f>B70*$A$78</f>
-        <v>4705075.1790824905</v>
+        <v>15</v>
+      </c>
+      <c r="B88" t="e">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(B38 / $A$82) - 1) - $B$74)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="C88">
-        <f>C70*$A$78</f>
-        <v>1845212.6988639566</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(C38 / $A$82) - 1) - $B$74)</f>
+        <v>247346.46896072372</v>
       </c>
       <c r="D88">
-        <f>D70*$A$78</f>
-        <v>1239376.6670631077</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(D38 / $A$82) - 1) - $B$74)</f>
+        <v>538051.58533345419</v>
       </c>
       <c r="E88">
-        <f>E70*$A$78</f>
-        <v>777645.80891369865</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(E38 / $A$82) - 1) - $B$74)</f>
+        <v>1090391.6731337465</v>
       </c>
       <c r="F88">
-        <f>F70*$A$78</f>
-        <v>222458.2765115248</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(F38 / $A$82) - 1) - $B$74)</f>
+        <v>2378646.8734586448</v>
       </c>
       <c r="G88">
-        <f>G70*$A$78</f>
-        <v>108788.88659203613</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(G38 / $A$82) - 1) - $B$74)</f>
+        <v>2287634.7382267094</v>
       </c>
       <c r="H88">
-        <f>H70*$A$78</f>
-        <v>31257.406209767105</v>
-      </c>
-      <c r="I88" t="e">
-        <f>I70*$A$78</f>
-        <v>#DIV/0!</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(H38 / $A$82) - 1) - $B$74)</f>
+        <v>1947785.5811512677</v>
+      </c>
+      <c r="I88">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(I38 / $A$82) - 1) - $B$74)</f>
+        <v>1729495.116710223</v>
       </c>
       <c r="J88">
-        <f>J70*$A$78</f>
-        <v>15118.752139782853</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(J38 / $A$82) - 1) - $B$74)</f>
+        <v>1613152.90395498</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B89">
-        <f>B71*$A$78</f>
-        <v>4416246.0319977961</v>
-      </c>
-      <c r="C89">
-        <f>C71*$A$78</f>
-        <v>1765850.7560394011</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(B39 / $A$82) - 1) - $B$74)</f>
+        <v>247346.46896072372</v>
+      </c>
+      <c r="C89" t="e">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(C39 / $A$82) - 1) - $B$74)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="D89">
-        <f>D71*$A$78</f>
-        <v>1198393.1066525034</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(D39 / $A$82) - 1) - $B$74)</f>
+        <v>53965.767472904154</v>
       </c>
       <c r="E89">
-        <f>E71*$A$78</f>
-        <v>764017.5652462513</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(E39 / $A$82) - 1) - $B$74)</f>
+        <v>172099.2816381779</v>
       </c>
       <c r="F89">
-        <f>F71*$A$78</f>
-        <v>237315.28535437089</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(F39 / $A$82) - 1) - $B$74)</f>
+        <v>619398.60607401293</v>
       </c>
       <c r="G89">
-        <f>G71*$A$78</f>
-        <v>126697.88901616511</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(G39 / $A$82) - 1) - $B$74)</f>
+        <v>703019.20098253549</v>
       </c>
       <c r="H89">
-        <f>H71*$A$78</f>
-        <v>48315.598944627753</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(H39 / $A$82) - 1) - $B$74)</f>
+        <v>681175.17348077009</v>
       </c>
       <c r="I89">
-        <f>I71*$A$78</f>
-        <v>15118.752139782853</v>
-      </c>
-      <c r="J89" t="e">
-        <f>J71*$A$78</f>
-        <v>#DIV/0!</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(I39 / $A$82) - 1) - $B$74)</f>
+        <v>638397.20927423215</v>
+      </c>
+      <c r="J89">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(J39 / $A$82) - 1) - $B$74)</f>
+        <v>609945.07659356785</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(B40 / $A$82) - 1) - $B$74)</f>
+        <v>538051.58533345419</v>
+      </c>
+      <c r="C90">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(C40 / $A$82) - 1) - $B$74)</f>
+        <v>53965.767472904154</v>
+      </c>
+      <c r="D90" t="e">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(D40 / $A$82) - 1) - $B$74)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E90">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(E40 / $A$82) - 1) - $B$74)</f>
+        <v>59885.217399664092</v>
+      </c>
+      <c r="F90">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(F40 / $A$82) - 1) - $B$74)</f>
+        <v>342164.43247450946</v>
+      </c>
+      <c r="G90">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(G40 / $A$82) - 1) - $B$74)</f>
+        <v>425657.46059352753</v>
+      </c>
+      <c r="H90">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(H40 / $A$82) - 1) - $B$74)</f>
+        <v>440332.17041074706</v>
+      </c>
+      <c r="I90">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(I40 / $A$82) - 1) - $B$74)</f>
+        <v>423519.621772215</v>
+      </c>
+      <c r="J90">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(J40 / $A$82) - 1) - $B$74)</f>
+        <v>409174.30282323126</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" t="s">
-        <v>41</v>
-      </c>
-      <c r="B91" t="s">
-        <v>15</v>
-      </c>
-      <c r="C91" t="s">
-        <v>16</v>
-      </c>
-      <c r="D91" t="s">
-        <v>17</v>
-      </c>
-      <c r="E91" t="s">
-        <v>18</v>
-      </c>
-      <c r="F91" t="s">
-        <v>4</v>
-      </c>
-      <c r="G91" t="s">
-        <v>19</v>
-      </c>
-      <c r="H91" t="s">
-        <v>20</v>
-      </c>
-      <c r="I91" t="s">
-        <v>21</v>
-      </c>
-      <c r="J91" t="s">
-        <v>22</v>
+        <v>3</v>
+      </c>
+      <c r="B91">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(B41 / $A$82) - 1) - $B$74)</f>
+        <v>1090391.6731337465</v>
+      </c>
+      <c r="C91">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(C41 / $A$82) - 1) - $B$74)</f>
+        <v>172099.2816381779</v>
+      </c>
+      <c r="D91">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(D41 / $A$82) - 1) - $B$74)</f>
+        <v>59885.217399664092</v>
+      </c>
+      <c r="E91" t="e">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(E41 / $A$82) - 1) - $B$74)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F91">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(F41 / $A$82) - 1) - $B$74)</f>
+        <v>160327.49729596975</v>
+      </c>
+      <c r="G91">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(G41 / $A$82) - 1) - $B$74)</f>
+        <v>230606.66594038581</v>
+      </c>
+      <c r="H91">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(H41 / $A$82) - 1) - $B$74)</f>
+        <v>263333.52332451061</v>
+      </c>
+      <c r="I91">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(I41 / $A$82) - 1) - $B$74)</f>
+        <v>263269.33488319488</v>
+      </c>
+      <c r="J91">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(J41 / $A$82) - 1) - $B$74)</f>
+        <v>258584.66483865233</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" t="s">
-        <v>15</v>
-      </c>
-      <c r="B92" t="e">
-        <f>$A$76-B81</f>
-        <v>#DIV/0!</v>
+        <v>4</v>
+      </c>
+      <c r="B92">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(B42 / $A$82) - 1) - $B$74)</f>
+        <v>2378646.8734586448</v>
       </c>
       <c r="C92">
-        <f t="shared" ref="C92:J92" si="32">$A$76-C81</f>
-        <v>18706.11550022033</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(C42 / $A$82) - 1) - $B$74)</f>
+        <v>619398.60607401293</v>
       </c>
       <c r="D92">
-        <f t="shared" si="32"/>
-        <v>-814158.82709165104</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(D42 / $A$82) - 1) - $B$74)</f>
+        <v>342164.43247450946</v>
       </c>
       <c r="E92">
-        <f t="shared" si="32"/>
-        <v>-2322172.7472044011</v>
-      </c>
-      <c r="F92">
-        <f t="shared" si="32"/>
-        <v>-5502435.5020517446</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(E42 / $A$82) - 1) - $B$74)</f>
+        <v>160327.49729596975</v>
+      </c>
+      <c r="F92" t="e">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(F42 / $A$82) - 1) - $B$74)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="G92">
-        <f t="shared" si="32"/>
-        <v>-5291825.5941903954</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(G42 / $A$82) - 1) - $B$74)</f>
+        <v>30138.575621783679</v>
       </c>
       <c r="H92">
-        <f t="shared" si="32"/>
-        <v>-4487343.5414584484</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(H42 / $A$82) - 1) - $B$74)</f>
+        <v>61262.445900102692</v>
       </c>
       <c r="I92">
-        <f t="shared" si="32"/>
-        <v>-3955075.1790824905</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(I42 / $A$82) - 1) - $B$74)</f>
+        <v>74480.855525358595</v>
       </c>
       <c r="J92">
-        <f t="shared" si="32"/>
-        <v>-3666246.0319977961</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(J42 / $A$82) - 1) - $B$74)</f>
+        <v>79478.589855372949</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B93">
-        <f t="shared" ref="B93:J93" si="33">$A$76-B82</f>
-        <v>18706.11550022033</v>
-      </c>
-      <c r="C93" t="e">
-        <f t="shared" si="33"/>
-        <v>#DIV/0!</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(B43 / $A$82) - 1) - $B$74)</f>
+        <v>2287634.7382267094</v>
+      </c>
+      <c r="C93">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(C43 / $A$82) - 1) - $B$74)</f>
+        <v>703019.20098253549</v>
       </c>
       <c r="D93">
-        <f t="shared" si="33"/>
-        <v>588620.06345043366</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(D43 / $A$82) - 1) - $B$74)</f>
+        <v>425657.46059352753</v>
       </c>
       <c r="E93">
-        <f t="shared" si="33"/>
-        <v>238927.21993579553</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(E43 / $A$82) - 1) - $B$74)</f>
+        <v>230606.66594038581</v>
       </c>
       <c r="F93">
-        <f t="shared" si="33"/>
-        <v>-1042248.3262411146</v>
-      </c>
-      <c r="G93">
-        <f t="shared" si="33"/>
-        <v>-1274507.0678264096</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(F43 / $A$82) - 1) - $B$74)</f>
+        <v>30138.575621783679</v>
+      </c>
+      <c r="G93" t="e">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(G43 / $A$82) - 1) - $B$74)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="H93">
-        <f t="shared" si="33"/>
-        <v>-1214048.6198853746</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(H43 / $A$82) - 1) - $B$74)</f>
+        <v>23530.265828788499</v>
       </c>
       <c r="I93">
-        <f t="shared" si="33"/>
-        <v>-1095212.6988639566</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(I43 / $A$82) - 1) - $B$74)</f>
+        <v>36341.249803354687</v>
       </c>
       <c r="J93">
-        <f t="shared" si="33"/>
-        <v>-1015850.7560394011</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(J43 / $A$82) - 1) - $B$74)</f>
+        <v>42338.852309897244</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B94">
-        <f t="shared" ref="B94:J94" si="34">$A$76-B83</f>
-        <v>-814158.82709165104</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(B44 / $A$82) - 1) - $B$74)</f>
+        <v>1947785.5811512677</v>
       </c>
       <c r="C94">
-        <f t="shared" si="34"/>
-        <v>588620.06345043366</v>
-      </c>
-      <c r="D94" t="e">
-        <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(C44 / $A$82) - 1) - $B$74)</f>
+        <v>681175.17348077009</v>
+      </c>
+      <c r="D94">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(D44 / $A$82) - 1) - $B$74)</f>
+        <v>440332.17041074706</v>
       </c>
       <c r="E94">
-        <f t="shared" si="34"/>
-        <v>570981.21387580014</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(E44 / $A$82) - 1) - $B$74)</f>
+        <v>263333.52332451061</v>
       </c>
       <c r="F94">
-        <f t="shared" si="34"/>
-        <v>-256043.84662210708</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(F44 / $A$82) - 1) - $B$74)</f>
+        <v>61262.445900102692</v>
       </c>
       <c r="G94">
-        <f t="shared" si="34"/>
-        <v>-495478.48808964575</v>
-      </c>
-      <c r="H94">
-        <f t="shared" si="34"/>
-        <v>-537322.28842354799</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(G44 / $A$82) - 1) - $B$74)</f>
+        <v>23530.265828788499</v>
+      </c>
+      <c r="H94" t="e">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(H44 / $A$82) - 1) - $B$74)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I94">
-        <f t="shared" si="34"/>
-        <v>-489376.66706310771</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(I44 / $A$82) - 1) - $B$74)</f>
+        <v>10425.5884102243</v>
       </c>
       <c r="J94">
-        <f t="shared" si="34"/>
-        <v>-448393.10665250337</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(J44 / $A$82) - 1) - $B$74)</f>
+        <v>16120.622966109609</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B95">
-        <f t="shared" ref="B95:J95" si="35">$A$76-B84</f>
-        <v>-2322172.7472044011</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(B45 / $A$82) - 1) - $B$74)</f>
+        <v>1729495.116710223</v>
       </c>
       <c r="C95">
-        <f t="shared" si="35"/>
-        <v>238927.21993579553</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(C45 / $A$82) - 1) - $B$74)</f>
+        <v>638397.20927423215</v>
       </c>
       <c r="D95">
-        <f t="shared" si="35"/>
-        <v>570981.21387580014</v>
-      </c>
-      <c r="E95" t="e">
-        <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(D45 / $A$82) - 1) - $B$74)</f>
+        <v>423519.621772215</v>
+      </c>
+      <c r="E95">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(E45 / $A$82) - 1) - $B$74)</f>
+        <v>263269.33488319488</v>
       </c>
       <c r="F95">
-        <f t="shared" si="35"/>
-        <v>273555.36019329599</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(F45 / $A$82) - 1) - $B$74)</f>
+        <v>74480.855525358595</v>
       </c>
       <c r="G95">
-        <f t="shared" si="35"/>
-        <v>67529.443347483175</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(G45 / $A$82) - 1) - $B$74)</f>
+        <v>36341.249803354687</v>
       </c>
       <c r="H95">
-        <f t="shared" si="35"/>
-        <v>-27832.488600495621</v>
-      </c>
-      <c r="I95">
-        <f t="shared" si="35"/>
-        <v>-27645.808913698653</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(H45 / $A$82) - 1) - $B$74)</f>
+        <v>10425.5884102243</v>
+      </c>
+      <c r="I95" t="e">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(I45 / $A$82) - 1) - $B$74)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="J95">
-        <f t="shared" si="35"/>
-        <v>-14017.565246251295</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(J45 / $A$82) - 1) - $B$74)</f>
+        <v>5041.093255296073</v>
       </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B96">
-        <f t="shared" ref="B96:J96" si="36">$A$76-B85</f>
-        <v>-5502435.5020517446</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(B46 / $A$82) - 1) - $B$74)</f>
+        <v>1613152.90395498</v>
       </c>
       <c r="C96">
-        <f t="shared" si="36"/>
-        <v>-1042248.3262411146</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(C46 / $A$82) - 1) - $B$74)</f>
+        <v>609945.07659356785</v>
       </c>
       <c r="D96">
-        <f t="shared" si="36"/>
-        <v>-256043.84662210708</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(D46 / $A$82) - 1) - $B$74)</f>
+        <v>409174.30282323126</v>
       </c>
       <c r="E96">
-        <f t="shared" si="36"/>
-        <v>273555.36019329599</v>
-      </c>
-      <c r="F96" t="e">
-        <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(E46 / $A$82) - 1) - $B$74)</f>
+        <v>258584.66483865233</v>
+      </c>
+      <c r="F96">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(F46 / $A$82) - 1) - $B$74)</f>
+        <v>79478.589855372949</v>
       </c>
       <c r="G96">
-        <f t="shared" si="36"/>
-        <v>659745.86507943005</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(G46 / $A$82) - 1) - $B$74)</f>
+        <v>42338.852309897244</v>
       </c>
       <c r="H96">
-        <f t="shared" si="36"/>
-        <v>566879.10392280726</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(H46 / $A$82) - 1) - $B$74)</f>
+        <v>16120.622966109609</v>
       </c>
       <c r="I96">
-        <f t="shared" si="36"/>
-        <v>527541.7234884752</v>
-      </c>
-      <c r="J96">
-        <f t="shared" si="36"/>
-        <v>512684.71464562911</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10">
-      <c r="A97" t="s">
-        <v>5</v>
-      </c>
-      <c r="B97">
-        <f t="shared" ref="B97:J97" si="37">$A$76-B86</f>
-        <v>-5291825.5941903954</v>
-      </c>
-      <c r="C97">
-        <f t="shared" si="37"/>
-        <v>-1274507.0678264096</v>
-      </c>
-      <c r="D97">
-        <f t="shared" si="37"/>
-        <v>-495478.48808964575</v>
-      </c>
-      <c r="E97">
-        <f t="shared" si="37"/>
-        <v>67529.443347483175</v>
-      </c>
-      <c r="F97">
-        <f t="shared" si="37"/>
-        <v>659745.86507943005</v>
-      </c>
-      <c r="G97" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H97">
-        <f t="shared" si="37"/>
-        <v>679507.739244394</v>
-      </c>
-      <c r="I97">
-        <f t="shared" si="37"/>
-        <v>641211.11340796389</v>
-      </c>
-      <c r="J97">
-        <f t="shared" si="37"/>
-        <v>623302.11098383483</v>
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(I46 / $A$82) - 1) - $B$74)</f>
+        <v>5041.093255296073</v>
+      </c>
+      <c r="J96" t="e">
+        <f>$A$84 * (1+$B$73) / ( 1 / (EXP(J46 / $A$82) - 1) - $B$74)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" t="s">
-        <v>6</v>
-      </c>
-      <c r="B98">
-        <f t="shared" ref="B98:J98" si="38">$A$76-B87</f>
-        <v>-4487343.5414584484</v>
-      </c>
-      <c r="C98">
-        <f t="shared" si="38"/>
-        <v>-1214048.6198853746</v>
-      </c>
-      <c r="D98">
-        <f t="shared" si="38"/>
-        <v>-537322.28842354799</v>
-      </c>
-      <c r="E98">
-        <f t="shared" si="38"/>
-        <v>-27832.488600495621</v>
-      </c>
-      <c r="F98">
-        <f t="shared" si="38"/>
-        <v>566879.10392280726</v>
-      </c>
-      <c r="G98">
-        <f t="shared" si="38"/>
-        <v>679507.739244394</v>
-      </c>
-      <c r="H98" t="e">
-        <f t="shared" si="38"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I98">
-        <f t="shared" si="38"/>
-        <v>718742.5937902329</v>
-      </c>
-      <c r="J98">
-        <f t="shared" si="38"/>
-        <v>701684.4010553722</v>
+        <v>36</v>
       </c>
     </row>
     <row r="99" spans="1:10">
-      <c r="A99" t="s">
-        <v>7</v>
-      </c>
-      <c r="B99">
-        <f t="shared" ref="B99:J99" si="39">$A$76-B88</f>
-        <v>-3955075.1790824905</v>
-      </c>
-      <c r="C99">
-        <f t="shared" si="39"/>
-        <v>-1095212.6988639566</v>
-      </c>
-      <c r="D99">
-        <f t="shared" si="39"/>
-        <v>-489376.66706310771</v>
-      </c>
-      <c r="E99">
-        <f t="shared" si="39"/>
-        <v>-27645.808913698653</v>
-      </c>
-      <c r="F99">
-        <f t="shared" si="39"/>
-        <v>527541.7234884752</v>
-      </c>
-      <c r="G99">
-        <f t="shared" si="39"/>
-        <v>641211.11340796389</v>
-      </c>
-      <c r="H99">
-        <f t="shared" si="39"/>
-        <v>718742.5937902329</v>
-      </c>
-      <c r="I99" t="e">
-        <f t="shared" si="39"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J99">
-        <f t="shared" si="39"/>
-        <v>734881.24786021712</v>
+      <c r="A99">
+        <v>15</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101">
+        <f>A99*A84</f>
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" t="s">
+        <v>39</v>
+      </c>
+      <c r="B105" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" t="s">
+        <v>16</v>
+      </c>
+      <c r="D105" t="s">
+        <v>17</v>
+      </c>
+      <c r="E105" t="s">
+        <v>18</v>
+      </c>
+      <c r="F105" t="s">
+        <v>4</v>
+      </c>
+      <c r="G105" t="s">
+        <v>19</v>
+      </c>
+      <c r="H105" t="s">
+        <v>20</v>
+      </c>
+      <c r="I105" t="s">
+        <v>21</v>
+      </c>
+      <c r="J105" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" t="s">
+        <v>15</v>
+      </c>
+      <c r="B106" t="e">
+        <f>B88*$A$103</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C106">
+        <f>C88*$A$103</f>
+        <v>742039.40688217117</v>
+      </c>
+      <c r="D106">
+        <f>D88*$A$103</f>
+        <v>1614154.7560003626</v>
+      </c>
+      <c r="E106">
+        <f>E88*$A$103</f>
+        <v>3271175.0194012392</v>
+      </c>
+      <c r="F106">
+        <f>F88*$A$103</f>
+        <v>7135940.620375935</v>
+      </c>
+      <c r="G106">
+        <f>G88*$A$103</f>
+        <v>6862904.2146801278</v>
+      </c>
+      <c r="H106">
+        <f>H88*$A$103</f>
+        <v>5843356.7434538035</v>
+      </c>
+      <c r="I106">
+        <f>I88*$A$103</f>
+        <v>5188485.3501306688</v>
+      </c>
+      <c r="J106">
+        <f>J88*$A$103</f>
+        <v>4839458.7118649399</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" t="s">
+        <v>1</v>
+      </c>
+      <c r="B107">
+        <f>B89*$A$103</f>
+        <v>742039.40688217117</v>
+      </c>
+      <c r="C107" t="e">
+        <f>C89*$A$103</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D107">
+        <f>D89*$A$103</f>
+        <v>161897.30241871247</v>
+      </c>
+      <c r="E107">
+        <f>E89*$A$103</f>
+        <v>516297.84491453366</v>
+      </c>
+      <c r="F107">
+        <f>F89*$A$103</f>
+        <v>1858195.8182220389</v>
+      </c>
+      <c r="G107">
+        <f>G89*$A$103</f>
+        <v>2109057.6029476067</v>
+      </c>
+      <c r="H107">
+        <f>H89*$A$103</f>
+        <v>2043525.5204423103</v>
+      </c>
+      <c r="I107">
+        <f>I89*$A$103</f>
+        <v>1915191.6278226965</v>
+      </c>
+      <c r="J107">
+        <f>J89*$A$103</f>
+        <v>1829835.2297807036</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108">
+        <f>B90*$A$103</f>
+        <v>1614154.7560003626</v>
+      </c>
+      <c r="C108">
+        <f>C90*$A$103</f>
+        <v>161897.30241871247</v>
+      </c>
+      <c r="D108" t="e">
+        <f>D90*$A$103</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E108">
+        <f>E90*$A$103</f>
+        <v>179655.65219899226</v>
+      </c>
+      <c r="F108">
+        <f>F90*$A$103</f>
+        <v>1026493.2974235284</v>
+      </c>
+      <c r="G108">
+        <f>G90*$A$103</f>
+        <v>1276972.3817805825</v>
+      </c>
+      <c r="H108">
+        <f>H90*$A$103</f>
+        <v>1320996.5112322411</v>
+      </c>
+      <c r="I108">
+        <f>I90*$A$103</f>
+        <v>1270558.865316645</v>
+      </c>
+      <c r="J108">
+        <f>J90*$A$103</f>
+        <v>1227522.9084696937</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" t="s">
+        <v>3</v>
+      </c>
+      <c r="B109">
+        <f>B91*$A$103</f>
+        <v>3271175.0194012392</v>
+      </c>
+      <c r="C109">
+        <f>C91*$A$103</f>
+        <v>516297.84491453366</v>
+      </c>
+      <c r="D109">
+        <f>D91*$A$103</f>
+        <v>179655.65219899226</v>
+      </c>
+      <c r="E109" t="e">
+        <f>E91*$A$103</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F109">
+        <f>F91*$A$103</f>
+        <v>480982.49188790924</v>
+      </c>
+      <c r="G109">
+        <f>G91*$A$103</f>
+        <v>691819.99782115745</v>
+      </c>
+      <c r="H109">
+        <f>H91*$A$103</f>
+        <v>790000.56997353188</v>
+      </c>
+      <c r="I109">
+        <f>I91*$A$103</f>
+        <v>789808.00464958465</v>
+      </c>
+      <c r="J109">
+        <f>J91*$A$103</f>
+        <v>775753.99451595696</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110" t="s">
+        <v>4</v>
+      </c>
+      <c r="B110">
+        <f>B92*$A$103</f>
+        <v>7135940.620375935</v>
+      </c>
+      <c r="C110">
+        <f>C92*$A$103</f>
+        <v>1858195.8182220389</v>
+      </c>
+      <c r="D110">
+        <f>D92*$A$103</f>
+        <v>1026493.2974235284</v>
+      </c>
+      <c r="E110">
+        <f>E92*$A$103</f>
+        <v>480982.49188790924</v>
+      </c>
+      <c r="F110" t="e">
+        <f>F92*$A$103</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G110">
+        <f>G92*$A$103</f>
+        <v>90415.72686535104</v>
+      </c>
+      <c r="H110">
+        <f>H92*$A$103</f>
+        <v>183787.33770030807</v>
+      </c>
+      <c r="I110">
+        <f>I92*$A$103</f>
+        <v>223442.5665760758</v>
+      </c>
+      <c r="J110">
+        <f>J92*$A$103</f>
+        <v>238435.76956611883</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" t="s">
+        <v>5</v>
+      </c>
+      <c r="B111">
+        <f>B93*$A$103</f>
+        <v>6862904.2146801278</v>
+      </c>
+      <c r="C111">
+        <f>C93*$A$103</f>
+        <v>2109057.6029476067</v>
+      </c>
+      <c r="D111">
+        <f>D93*$A$103</f>
+        <v>1276972.3817805825</v>
+      </c>
+      <c r="E111">
+        <f>E93*$A$103</f>
+        <v>691819.99782115745</v>
+      </c>
+      <c r="F111">
+        <f>F93*$A$103</f>
+        <v>90415.72686535104</v>
+      </c>
+      <c r="G111" t="e">
+        <f>G93*$A$103</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H111">
+        <f>H93*$A$103</f>
+        <v>70590.797486365496</v>
+      </c>
+      <c r="I111">
+        <f>I93*$A$103</f>
+        <v>109023.74941006406</v>
+      </c>
+      <c r="J111">
+        <f>J93*$A$103</f>
+        <v>127016.55692969172</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112">
+        <f>B94*$A$103</f>
+        <v>5843356.7434538035</v>
+      </c>
+      <c r="C112">
+        <f>C94*$A$103</f>
+        <v>2043525.5204423103</v>
+      </c>
+      <c r="D112">
+        <f>D94*$A$103</f>
+        <v>1320996.5112322411</v>
+      </c>
+      <c r="E112">
+        <f>E94*$A$103</f>
+        <v>790000.56997353188</v>
+      </c>
+      <c r="F112">
+        <f>F94*$A$103</f>
+        <v>183787.33770030807</v>
+      </c>
+      <c r="G112">
+        <f>G94*$A$103</f>
+        <v>70590.797486365496</v>
+      </c>
+      <c r="H112" t="e">
+        <f>H94*$A$103</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I112">
+        <f>I94*$A$103</f>
+        <v>31276.7652306729</v>
+      </c>
+      <c r="J112">
+        <f>J94*$A$103</f>
+        <v>48361.86889832883</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113" t="s">
+        <v>7</v>
+      </c>
+      <c r="B113">
+        <f>B95*$A$103</f>
+        <v>5188485.3501306688</v>
+      </c>
+      <c r="C113">
+        <f>C95*$A$103</f>
+        <v>1915191.6278226965</v>
+      </c>
+      <c r="D113">
+        <f>D95*$A$103</f>
+        <v>1270558.865316645</v>
+      </c>
+      <c r="E113">
+        <f>E95*$A$103</f>
+        <v>789808.00464958465</v>
+      </c>
+      <c r="F113">
+        <f>F95*$A$103</f>
+        <v>223442.5665760758</v>
+      </c>
+      <c r="G113">
+        <f>G95*$A$103</f>
+        <v>109023.74941006406</v>
+      </c>
+      <c r="H113">
+        <f>H95*$A$103</f>
+        <v>31276.7652306729</v>
+      </c>
+      <c r="I113" t="e">
+        <f>I95*$A$103</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J113">
+        <f>J95*$A$103</f>
+        <v>15123.279765888219</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" t="s">
         <v>13</v>
       </c>
-      <c r="B100">
-        <f t="shared" ref="B100:J100" si="40">$A$76-B89</f>
-        <v>-3666246.0319977961</v>
-      </c>
-      <c r="C100">
-        <f t="shared" si="40"/>
-        <v>-1015850.7560394011</v>
-      </c>
-      <c r="D100">
-        <f t="shared" si="40"/>
-        <v>-448393.10665250337</v>
-      </c>
-      <c r="E100">
-        <f t="shared" si="40"/>
-        <v>-14017.565246251295</v>
-      </c>
-      <c r="F100">
-        <f t="shared" si="40"/>
-        <v>512684.71464562911</v>
-      </c>
-      <c r="G100">
-        <f t="shared" si="40"/>
-        <v>623302.11098383483</v>
-      </c>
-      <c r="H100">
-        <f t="shared" si="40"/>
-        <v>701684.4010553722</v>
-      </c>
-      <c r="I100">
-        <f t="shared" si="40"/>
-        <v>734881.24786021712</v>
-      </c>
-      <c r="J100" t="e">
-        <f t="shared" si="40"/>
+      <c r="B114">
+        <f>B96*$A$103</f>
+        <v>4839458.7118649399</v>
+      </c>
+      <c r="C114">
+        <f>C96*$A$103</f>
+        <v>1829835.2297807036</v>
+      </c>
+      <c r="D114">
+        <f>D96*$A$103</f>
+        <v>1227522.9084696937</v>
+      </c>
+      <c r="E114">
+        <f>E96*$A$103</f>
+        <v>775753.99451595696</v>
+      </c>
+      <c r="F114">
+        <f>F96*$A$103</f>
+        <v>238435.76956611883</v>
+      </c>
+      <c r="G114">
+        <f>G96*$A$103</f>
+        <v>127016.55692969172</v>
+      </c>
+      <c r="H114">
+        <f>H96*$A$103</f>
+        <v>48361.86889832883</v>
+      </c>
+      <c r="I114">
+        <f>I96*$A$103</f>
+        <v>15123.279765888219</v>
+      </c>
+      <c r="J114" t="e">
+        <f>J96*$A$103</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" t="s">
+        <v>45</v>
+      </c>
+      <c r="B116" t="s">
+        <v>15</v>
+      </c>
+      <c r="C116" t="s">
+        <v>16</v>
+      </c>
+      <c r="D116" t="s">
+        <v>17</v>
+      </c>
+      <c r="E116" t="s">
+        <v>18</v>
+      </c>
+      <c r="F116" t="s">
+        <v>4</v>
+      </c>
+      <c r="G116" t="s">
+        <v>19</v>
+      </c>
+      <c r="H116" t="s">
+        <v>20</v>
+      </c>
+      <c r="I116" t="s">
+        <v>21</v>
+      </c>
+      <c r="J116" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" t="s">
+        <v>15</v>
+      </c>
+      <c r="B117">
+        <f>$B$70*$B$71*B60</f>
+        <v>17593.697845566283</v>
+      </c>
+      <c r="C117">
+        <f t="shared" ref="C117:J117" si="48">$B$70*$B$71*C60</f>
+        <v>30221.604932417125</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="48"/>
+        <v>42193.102700583047</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="48"/>
+        <v>68217.492525337046</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="48"/>
+        <v>341486.08001483028</v>
+      </c>
+      <c r="G117">
+        <f t="shared" si="48"/>
+        <v>813024.71686986496</v>
+      </c>
+      <c r="H117">
+        <f t="shared" si="48"/>
+        <v>2242061.7101087561</v>
+      </c>
+      <c r="I117">
+        <f t="shared" si="48"/>
+        <v>4349792.2725010235</v>
+      </c>
+      <c r="J117">
+        <f t="shared" si="48"/>
+        <v>6501337.022223359</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" t="s">
+        <v>1</v>
+      </c>
+      <c r="B118">
+        <f t="shared" ref="B118:J118" si="49">$B$70*$B$71*B61</f>
+        <v>30221.604932417125</v>
+      </c>
+      <c r="C118">
+        <f t="shared" si="49"/>
+        <v>44939.915944559696</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="49"/>
+        <v>58429.769485110373</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="49"/>
+        <v>86993.848137140259</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="49"/>
+        <v>372746.50929601822</v>
+      </c>
+      <c r="G118">
+        <f t="shared" si="49"/>
+        <v>854499.18591786514</v>
+      </c>
+      <c r="H118">
+        <f t="shared" si="49"/>
+        <v>2299985.285276758</v>
+      </c>
+      <c r="I118">
+        <f t="shared" si="49"/>
+        <v>4421925.621122973</v>
+      </c>
+      <c r="J118">
+        <f t="shared" si="49"/>
+        <v>6583757.3607811239</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" t="s">
+        <v>2</v>
+      </c>
+      <c r="B119">
+        <f t="shared" ref="B119:J119" si="50">$B$70*$B$71*B62</f>
+        <v>42193.102700583047</v>
+      </c>
+      <c r="C119">
+        <f t="shared" si="50"/>
+        <v>58429.769485110373</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="50"/>
+        <v>73050.92809294656</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="50"/>
+        <v>103545.66347891625</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="50"/>
+        <v>399144.75629591168</v>
+      </c>
+      <c r="G119">
+        <f t="shared" si="50"/>
+        <v>889138.2956472598</v>
+      </c>
+      <c r="H119">
+        <f t="shared" si="50"/>
+        <v>2348015.2915365016</v>
+      </c>
+      <c r="I119">
+        <f t="shared" si="50"/>
+        <v>4481575.9519538926</v>
+      </c>
+      <c r="J119">
+        <f t="shared" si="50"/>
+        <v>6651835.4936313266</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
+      <c r="A120" t="s">
+        <v>3</v>
+      </c>
+      <c r="B120">
+        <f t="shared" ref="B120:J120" si="51">$B$70*$B$71*B63</f>
+        <v>68217.492525337046</v>
+      </c>
+      <c r="C120">
+        <f t="shared" si="51"/>
+        <v>86993.848137140259</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="51"/>
+        <v>103545.66347891625</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="51"/>
+        <v>137393.42844763375</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="51"/>
+        <v>450730.93681354221</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="51"/>
+        <v>955946.55651884282</v>
+      </c>
+      <c r="H120">
+        <f t="shared" si="51"/>
+        <v>2439827.771786375</v>
+      </c>
+      <c r="I120">
+        <f t="shared" si="51"/>
+        <v>4595209.3238181751</v>
+      </c>
+      <c r="J120">
+        <f t="shared" si="51"/>
+        <v>6781331.606271876</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" t="s">
+        <v>4</v>
+      </c>
+      <c r="B121">
+        <f t="shared" ref="B121:J121" si="52">$B$70*$B$71*B64</f>
+        <v>341486.08001483028</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="52"/>
+        <v>372746.50929601822</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="52"/>
+        <v>399144.75629591168</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="52"/>
+        <v>450730.93681354221</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="52"/>
+        <v>867324.75118397828</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="52"/>
+        <v>1468590.9707013755</v>
+      </c>
+      <c r="H121">
+        <f t="shared" si="52"/>
+        <v>3117266.4392844983</v>
+      </c>
+      <c r="I121">
+        <f t="shared" si="52"/>
+        <v>5420114.8883930007</v>
+      </c>
+      <c r="J121">
+        <f t="shared" si="52"/>
+        <v>7714621.8084493885</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
+      <c r="A122" t="s">
+        <v>5</v>
+      </c>
+      <c r="B122">
+        <f t="shared" ref="B122:J122" si="53">$B$70*$B$71*B65</f>
+        <v>813024.71686986496</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="53"/>
+        <v>854499.18591786514</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="53"/>
+        <v>889138.2956472598</v>
+      </c>
+      <c r="E122">
+        <f t="shared" si="53"/>
+        <v>955946.55651884282</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="53"/>
+        <v>1468590.9707013755</v>
+      </c>
+      <c r="G122">
+        <f t="shared" si="53"/>
+        <v>2166959.4175449843</v>
+      </c>
+      <c r="H122">
+        <f t="shared" si="53"/>
+        <v>3992014.3627896658</v>
+      </c>
+      <c r="I122">
+        <f t="shared" si="53"/>
+        <v>6458699.3059591418</v>
+      </c>
+      <c r="J122">
+        <f t="shared" si="53"/>
+        <v>8875781.1095264927</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
+      <c r="A123" t="s">
+        <v>6</v>
+      </c>
+      <c r="B123">
+        <f t="shared" ref="B123:J123" si="54">$B$70*$B$71*B66</f>
+        <v>2242061.7101087561</v>
+      </c>
+      <c r="C123">
+        <f t="shared" si="54"/>
+        <v>2299985.285276758</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="54"/>
+        <v>2348015.2915365016</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="54"/>
+        <v>2439827.771786375</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="54"/>
+        <v>3117266.4392844983</v>
+      </c>
+      <c r="G123">
+        <f t="shared" si="54"/>
+        <v>3992014.3627896658</v>
+      </c>
+      <c r="H123">
+        <f t="shared" si="54"/>
+        <v>6154624.7693134025</v>
+      </c>
+      <c r="I123">
+        <f t="shared" si="54"/>
+        <v>8948006.4399637543</v>
+      </c>
+      <c r="J123">
+        <f t="shared" si="54"/>
+        <v>11615024.749328032</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
+      <c r="A124" t="s">
+        <v>7</v>
+      </c>
+      <c r="B124">
+        <f t="shared" ref="B124:J124" si="55">$B$70*$B$71*B67</f>
+        <v>4349792.2725010235</v>
+      </c>
+      <c r="C124">
+        <f t="shared" si="55"/>
+        <v>4421925.621122973</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="55"/>
+        <v>4481575.9519538926</v>
+      </c>
+      <c r="E124">
+        <f t="shared" si="55"/>
+        <v>4595209.3238181751</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="55"/>
+        <v>5420114.8883930007</v>
+      </c>
+      <c r="G124">
+        <f t="shared" si="55"/>
+        <v>6458699.3059591418</v>
+      </c>
+      <c r="H124">
+        <f t="shared" si="55"/>
+        <v>8948006.4399637543</v>
+      </c>
+      <c r="I124">
+        <f t="shared" si="55"/>
+        <v>12069572.037552707</v>
+      </c>
+      <c r="J124">
+        <f t="shared" si="55"/>
+        <v>14993430.09486215</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
+      <c r="A125" t="s">
+        <v>13</v>
+      </c>
+      <c r="B125">
+        <f t="shared" ref="B125:J125" si="56">$B$70*$B$71*B68</f>
+        <v>6501337.022223359</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="56"/>
+        <v>6583757.3607811239</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="56"/>
+        <v>6651835.4936313266</v>
+      </c>
+      <c r="E125">
+        <f t="shared" si="56"/>
+        <v>6781331.606271876</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="56"/>
+        <v>7714621.8084493885</v>
+      </c>
+      <c r="G125">
+        <f t="shared" si="56"/>
+        <v>8875781.1095264927</v>
+      </c>
+      <c r="H125">
+        <f t="shared" si="56"/>
+        <v>11615024.749328032</v>
+      </c>
+      <c r="I125">
+        <f t="shared" si="56"/>
+        <v>14993430.09486215</v>
+      </c>
+      <c r="J125">
+        <f t="shared" si="56"/>
+        <v>18121387.778178569</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
+      <c r="A127" t="s">
+        <v>40</v>
+      </c>
+      <c r="B127" t="s">
+        <v>15</v>
+      </c>
+      <c r="C127" t="s">
+        <v>16</v>
+      </c>
+      <c r="D127" t="s">
+        <v>17</v>
+      </c>
+      <c r="E127" t="s">
+        <v>18</v>
+      </c>
+      <c r="F127" t="s">
+        <v>4</v>
+      </c>
+      <c r="G127" t="s">
+        <v>19</v>
+      </c>
+      <c r="H127" t="s">
+        <v>20</v>
+      </c>
+      <c r="I127" t="s">
+        <v>21</v>
+      </c>
+      <c r="J127" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
+      <c r="A128" t="s">
+        <v>15</v>
+      </c>
+      <c r="B128" t="e">
+        <f>$A$101-B106-B117</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C128">
+        <f t="shared" ref="C128:J128" si="57">$A$101-C106-C117</f>
+        <v>-22261.011814588295</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="57"/>
+        <v>-906347.85870094562</v>
+      </c>
+      <c r="E128">
+        <f t="shared" si="57"/>
+        <v>-2589392.5119265765</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="57"/>
+        <v>-6727426.7003907654</v>
+      </c>
+      <c r="G128">
+        <f t="shared" si="57"/>
+        <v>-6925928.9315499924</v>
+      </c>
+      <c r="H128">
+        <f t="shared" si="57"/>
+        <v>-7335418.4535625596</v>
+      </c>
+      <c r="I128">
+        <f t="shared" si="57"/>
+        <v>-8788277.6226316914</v>
+      </c>
+      <c r="J128">
+        <f t="shared" si="57"/>
+        <v>-10590795.734088298</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10">
+      <c r="A129" t="s">
+        <v>1</v>
+      </c>
+      <c r="B129">
+        <f t="shared" ref="B129:J129" si="58">$A$101-B107-B118</f>
+        <v>-22261.011814588295</v>
+      </c>
+      <c r="C129" t="e">
+        <f t="shared" si="58"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="58"/>
+        <v>529672.92809617706</v>
+      </c>
+      <c r="E129">
+        <f t="shared" si="58"/>
+        <v>146708.30694832606</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="58"/>
+        <v>-1480942.3275180571</v>
+      </c>
+      <c r="G129">
+        <f t="shared" si="58"/>
+        <v>-2213556.7888654717</v>
+      </c>
+      <c r="H129">
+        <f t="shared" si="58"/>
+        <v>-3593510.8057190683</v>
+      </c>
+      <c r="I129">
+        <f t="shared" si="58"/>
+        <v>-5587117.2489456693</v>
+      </c>
+      <c r="J129">
+        <f t="shared" si="58"/>
+        <v>-7663592.5905618276</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10">
+      <c r="A130" t="s">
+        <v>2</v>
+      </c>
+      <c r="B130">
+        <f t="shared" ref="B130:J130" si="59">$A$101-B108-B119</f>
+        <v>-906347.85870094562</v>
+      </c>
+      <c r="C130">
+        <f t="shared" si="59"/>
+        <v>529672.92809617706</v>
+      </c>
+      <c r="D130" t="e">
+        <f t="shared" si="59"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E130">
+        <f t="shared" si="59"/>
+        <v>466798.68432209152</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="59"/>
+        <v>-675638.05371944001</v>
+      </c>
+      <c r="G130">
+        <f t="shared" si="59"/>
+        <v>-1416110.6774278423</v>
+      </c>
+      <c r="H130">
+        <f t="shared" si="59"/>
+        <v>-2919011.8027687427</v>
+      </c>
+      <c r="I130">
+        <f t="shared" si="59"/>
+        <v>-5002134.8172705378</v>
+      </c>
+      <c r="J130">
+        <f t="shared" si="59"/>
+        <v>-7129358.4021010203</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10">
+      <c r="A131" t="s">
+        <v>3</v>
+      </c>
+      <c r="B131">
+        <f t="shared" ref="B131:J131" si="60">$A$101-B109-B120</f>
+        <v>-2589392.5119265765</v>
+      </c>
+      <c r="C131">
+        <f t="shared" si="60"/>
+        <v>146708.30694832606</v>
+      </c>
+      <c r="D131">
+        <f t="shared" si="60"/>
+        <v>466798.68432209152</v>
+      </c>
+      <c r="E131" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F131">
+        <f t="shared" si="60"/>
+        <v>-181713.42870145146</v>
+      </c>
+      <c r="G131">
+        <f t="shared" si="60"/>
+        <v>-897766.55434000026</v>
+      </c>
+      <c r="H131">
+        <f t="shared" si="60"/>
+        <v>-2479828.3417599071</v>
+      </c>
+      <c r="I131">
+        <f t="shared" si="60"/>
+        <v>-4635017.3284677602</v>
+      </c>
+      <c r="J131">
+        <f t="shared" si="60"/>
+        <v>-6807085.6007878333</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10">
+      <c r="A132" t="s">
+        <v>4</v>
+      </c>
+      <c r="B132">
+        <f t="shared" ref="B132:J132" si="61">$A$101-B110-B121</f>
+        <v>-6727426.7003907654</v>
+      </c>
+      <c r="C132">
+        <f t="shared" si="61"/>
+        <v>-1480942.3275180571</v>
+      </c>
+      <c r="D132">
+        <f t="shared" si="61"/>
+        <v>-675638.05371944001</v>
+      </c>
+      <c r="E132">
+        <f t="shared" si="61"/>
+        <v>-181713.42870145146</v>
+      </c>
+      <c r="F132" t="e">
+        <f t="shared" si="61"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G132">
+        <f t="shared" si="61"/>
+        <v>-809006.69756672659</v>
+      </c>
+      <c r="H132">
+        <f t="shared" si="61"/>
+        <v>-2551053.7769848062</v>
+      </c>
+      <c r="I132">
+        <f t="shared" si="61"/>
+        <v>-4893557.4549690764</v>
+      </c>
+      <c r="J132">
+        <f t="shared" si="61"/>
+        <v>-7203057.5780155072</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10">
+      <c r="A133" t="s">
+        <v>5</v>
+      </c>
+      <c r="B133">
+        <f t="shared" ref="B133:J133" si="62">$A$101-B111-B122</f>
+        <v>-6925928.9315499924</v>
+      </c>
+      <c r="C133">
+        <f t="shared" si="62"/>
+        <v>-2213556.7888654717</v>
+      </c>
+      <c r="D133">
+        <f t="shared" si="62"/>
+        <v>-1416110.6774278423</v>
+      </c>
+      <c r="E133">
+        <f t="shared" si="62"/>
+        <v>-897766.55434000026</v>
+      </c>
+      <c r="F133">
+        <f t="shared" si="62"/>
+        <v>-809006.69756672659</v>
+      </c>
+      <c r="G133" t="e">
+        <f t="shared" si="62"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H133">
+        <f t="shared" si="62"/>
+        <v>-3312605.1602760311</v>
+      </c>
+      <c r="I133">
+        <f t="shared" si="62"/>
+        <v>-5817723.0553692058</v>
+      </c>
+      <c r="J133">
+        <f t="shared" si="62"/>
+        <v>-8252797.6664561843</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10">
+      <c r="A134" t="s">
+        <v>6</v>
+      </c>
+      <c r="B134">
+        <f t="shared" ref="B134:J134" si="63">$A$101-B112-B123</f>
+        <v>-7335418.4535625596</v>
+      </c>
+      <c r="C134">
+        <f t="shared" si="63"/>
+        <v>-3593510.8057190683</v>
+      </c>
+      <c r="D134">
+        <f t="shared" si="63"/>
+        <v>-2919011.8027687427</v>
+      </c>
+      <c r="E134">
+        <f t="shared" si="63"/>
+        <v>-2479828.3417599071</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="63"/>
+        <v>-2551053.7769848062</v>
+      </c>
+      <c r="G134">
+        <f t="shared" si="63"/>
+        <v>-3312605.1602760311</v>
+      </c>
+      <c r="H134" t="e">
+        <f t="shared" si="63"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I134">
+        <f t="shared" si="63"/>
+        <v>-8229283.2051944267</v>
+      </c>
+      <c r="J134">
+        <f t="shared" si="63"/>
+        <v>-10913386.618226361</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10">
+      <c r="A135" t="s">
+        <v>7</v>
+      </c>
+      <c r="B135">
+        <f t="shared" ref="B135:J135" si="64">$A$101-B113-B124</f>
+        <v>-8788277.6226316914</v>
+      </c>
+      <c r="C135">
+        <f t="shared" si="64"/>
+        <v>-5587117.2489456693</v>
+      </c>
+      <c r="D135">
+        <f t="shared" si="64"/>
+        <v>-5002134.8172705378</v>
+      </c>
+      <c r="E135">
+        <f t="shared" si="64"/>
+        <v>-4635017.3284677602</v>
+      </c>
+      <c r="F135">
+        <f t="shared" si="64"/>
+        <v>-4893557.4549690764</v>
+      </c>
+      <c r="G135">
+        <f t="shared" si="64"/>
+        <v>-5817723.0553692058</v>
+      </c>
+      <c r="H135">
+        <f t="shared" si="64"/>
+        <v>-8229283.2051944267</v>
+      </c>
+      <c r="I135" t="e">
+        <f t="shared" si="64"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J135">
+        <f t="shared" si="64"/>
+        <v>-14258553.374628039</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10">
+      <c r="A136" t="s">
+        <v>13</v>
+      </c>
+      <c r="B136">
+        <f t="shared" ref="B136:J136" si="65">$A$101-B114-B125</f>
+        <v>-10590795.734088298</v>
+      </c>
+      <c r="C136">
+        <f t="shared" si="65"/>
+        <v>-7663592.5905618276</v>
+      </c>
+      <c r="D136">
+        <f t="shared" si="65"/>
+        <v>-7129358.4021010203</v>
+      </c>
+      <c r="E136">
+        <f t="shared" si="65"/>
+        <v>-6807085.6007878333</v>
+      </c>
+      <c r="F136">
+        <f t="shared" si="65"/>
+        <v>-7203057.5780155072</v>
+      </c>
+      <c r="G136">
+        <f t="shared" si="65"/>
+        <v>-8252797.6664561843</v>
+      </c>
+      <c r="H136">
+        <f t="shared" si="65"/>
+        <v>-10913386.618226361</v>
+      </c>
+      <c r="I136">
+        <f t="shared" si="65"/>
+        <v>-14258553.374628039</v>
+      </c>
+      <c r="J136" t="e">
+        <f t="shared" si="65"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10">
+      <c r="A138" t="s">
+        <v>47</v>
+      </c>
+      <c r="B138" t="s">
+        <v>15</v>
+      </c>
+      <c r="C138" t="s">
+        <v>16</v>
+      </c>
+      <c r="D138" t="s">
+        <v>17</v>
+      </c>
+      <c r="E138" t="s">
+        <v>18</v>
+      </c>
+      <c r="F138" t="s">
+        <v>4</v>
+      </c>
+      <c r="G138" t="s">
+        <v>19</v>
+      </c>
+      <c r="H138" t="s">
+        <v>20</v>
+      </c>
+      <c r="I138" t="s">
+        <v>21</v>
+      </c>
+      <c r="J138" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10">
+      <c r="A139" t="s">
+        <v>15</v>
+      </c>
+      <c r="B139" t="e">
+        <f>(B106+B117)/$A$84</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C139">
+        <f t="shared" ref="C139:J139" si="66">(C106+C117)/$A$84</f>
+        <v>15.445220236291767</v>
+      </c>
+      <c r="D139">
+        <f t="shared" si="66"/>
+        <v>33.126957174018912</v>
+      </c>
+      <c r="E139">
+        <f t="shared" si="66"/>
+        <v>66.787850238531533</v>
+      </c>
+      <c r="F139">
+        <f t="shared" si="66"/>
+        <v>149.54853400781531</v>
+      </c>
+      <c r="G139">
+        <f t="shared" si="66"/>
+        <v>153.51857863099985</v>
+      </c>
+      <c r="H139">
+        <f t="shared" si="66"/>
+        <v>161.70836907125118</v>
+      </c>
+      <c r="I139">
+        <f t="shared" si="66"/>
+        <v>190.76555245263384</v>
+      </c>
+      <c r="J139">
+        <f t="shared" si="66"/>
+        <v>226.81591468176595</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10">
+      <c r="A140" t="s">
+        <v>1</v>
+      </c>
+      <c r="B140">
+        <f t="shared" ref="B140:J140" si="67">(B107+B118)/$A$84</f>
+        <v>15.445220236291767</v>
+      </c>
+      <c r="C140" t="e">
+        <f t="shared" si="67"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D140">
+        <f t="shared" si="67"/>
+        <v>4.4065414380764567</v>
+      </c>
+      <c r="E140">
+        <f t="shared" si="67"/>
+        <v>12.065833861033479</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="67"/>
+        <v>44.618846550361141</v>
+      </c>
+      <c r="G140">
+        <f t="shared" si="67"/>
+        <v>59.271135777309432</v>
+      </c>
+      <c r="H140">
+        <f t="shared" si="67"/>
+        <v>86.870216114381364</v>
+      </c>
+      <c r="I140">
+        <f t="shared" si="67"/>
+        <v>126.74234497891338</v>
+      </c>
+      <c r="J140">
+        <f t="shared" si="67"/>
+        <v>168.27185181123656</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10">
+      <c r="A141" t="s">
+        <v>2</v>
+      </c>
+      <c r="B141">
+        <f t="shared" ref="B141:J141" si="68">(B108+B119)/$A$84</f>
+        <v>33.126957174018912</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="68"/>
+        <v>4.4065414380764567</v>
+      </c>
+      <c r="D141" t="e">
+        <f t="shared" si="68"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E141">
+        <f t="shared" si="68"/>
+        <v>5.6640263135581694</v>
+      </c>
+      <c r="F141">
+        <f t="shared" si="68"/>
+        <v>28.512761074388798</v>
+      </c>
+      <c r="G141">
+        <f t="shared" si="68"/>
+        <v>43.322213548556846</v>
+      </c>
+      <c r="H141">
+        <f t="shared" si="68"/>
+        <v>73.380236055374851</v>
+      </c>
+      <c r="I141">
+        <f t="shared" si="68"/>
+        <v>115.04269634541076</v>
+      </c>
+      <c r="J141">
+        <f t="shared" si="68"/>
+        <v>157.58716804202041</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10">
+      <c r="A142" t="s">
+        <v>3</v>
+      </c>
+      <c r="B142">
+        <f t="shared" ref="B142:J142" si="69">(B109+B120)/$A$84</f>
+        <v>66.787850238531533</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="69"/>
+        <v>12.065833861033479</v>
+      </c>
+      <c r="D142">
+        <f t="shared" si="69"/>
+        <v>5.6640263135581694</v>
+      </c>
+      <c r="E142" t="e">
+        <f t="shared" si="69"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F142">
+        <f t="shared" si="69"/>
+        <v>18.634268574029029</v>
+      </c>
+      <c r="G142">
+        <f t="shared" si="69"/>
+        <v>32.955331086800008</v>
+      </c>
+      <c r="H142">
+        <f t="shared" si="69"/>
+        <v>64.596566835198146</v>
+      </c>
+      <c r="I142">
+        <f t="shared" si="69"/>
+        <v>107.7003465693552</v>
+      </c>
+      <c r="J142">
+        <f t="shared" si="69"/>
+        <v>151.14171201575667</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10">
+      <c r="A143" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143">
+        <f t="shared" ref="B143:J143" si="70">(B110+B121)/$A$84</f>
+        <v>149.54853400781531</v>
+      </c>
+      <c r="C143">
+        <f t="shared" si="70"/>
+        <v>44.618846550361141</v>
+      </c>
+      <c r="D143">
+        <f t="shared" si="70"/>
+        <v>28.512761074388798</v>
+      </c>
+      <c r="E143">
+        <f t="shared" si="70"/>
+        <v>18.634268574029029</v>
+      </c>
+      <c r="F143" t="e">
+        <f t="shared" si="70"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G143">
+        <f t="shared" si="70"/>
+        <v>31.180133951334529</v>
+      </c>
+      <c r="H143">
+        <f t="shared" si="70"/>
+        <v>66.021075539696128</v>
+      </c>
+      <c r="I143">
+        <f t="shared" si="70"/>
+        <v>112.87114909938153</v>
+      </c>
+      <c r="J143">
+        <f t="shared" si="70"/>
+        <v>159.06115156031015</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10">
+      <c r="A144" t="s">
+        <v>5</v>
+      </c>
+      <c r="B144">
+        <f t="shared" ref="B144:J144" si="71">(B111+B122)/$A$84</f>
+        <v>153.51857863099985</v>
+      </c>
+      <c r="C144">
+        <f t="shared" si="71"/>
+        <v>59.271135777309432</v>
+      </c>
+      <c r="D144">
+        <f t="shared" si="71"/>
+        <v>43.322213548556846</v>
+      </c>
+      <c r="E144">
+        <f t="shared" si="71"/>
+        <v>32.955331086800008</v>
+      </c>
+      <c r="F144">
+        <f t="shared" si="71"/>
+        <v>31.180133951334529</v>
+      </c>
+      <c r="G144" t="e">
+        <f t="shared" si="71"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H144">
+        <f t="shared" si="71"/>
+        <v>81.252103205520626</v>
+      </c>
+      <c r="I144">
+        <f t="shared" si="71"/>
+        <v>131.35446110738411</v>
+      </c>
+      <c r="J144">
+        <f t="shared" si="71"/>
+        <v>180.0559533291237</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10">
+      <c r="A145" t="s">
+        <v>6</v>
+      </c>
+      <c r="B145">
+        <f t="shared" ref="B145:J145" si="72">(B112+B123)/$A$84</f>
+        <v>161.70836907125118</v>
+      </c>
+      <c r="C145">
+        <f t="shared" si="72"/>
+        <v>86.870216114381364</v>
+      </c>
+      <c r="D145">
+        <f t="shared" si="72"/>
+        <v>73.380236055374851</v>
+      </c>
+      <c r="E145">
+        <f t="shared" si="72"/>
+        <v>64.596566835198146</v>
+      </c>
+      <c r="F145">
+        <f t="shared" si="72"/>
+        <v>66.021075539696128</v>
+      </c>
+      <c r="G145">
+        <f t="shared" si="72"/>
+        <v>81.252103205520626</v>
+      </c>
+      <c r="H145" t="e">
+        <f t="shared" si="72"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I145">
+        <f t="shared" si="72"/>
+        <v>179.58566410388855</v>
+      </c>
+      <c r="J145">
+        <f t="shared" si="72"/>
+        <v>233.26773236452721</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10">
+      <c r="A146" t="s">
+        <v>7</v>
+      </c>
+      <c r="B146">
+        <f t="shared" ref="B146:J146" si="73">(B113+B124)/$A$84</f>
+        <v>190.76555245263384</v>
+      </c>
+      <c r="C146">
+        <f t="shared" si="73"/>
+        <v>126.74234497891338</v>
+      </c>
+      <c r="D146">
+        <f t="shared" si="73"/>
+        <v>115.04269634541076</v>
+      </c>
+      <c r="E146">
+        <f t="shared" si="73"/>
+        <v>107.7003465693552</v>
+      </c>
+      <c r="F146">
+        <f t="shared" si="73"/>
+        <v>112.87114909938153</v>
+      </c>
+      <c r="G146">
+        <f t="shared" si="73"/>
+        <v>131.35446110738411</v>
+      </c>
+      <c r="H146">
+        <f t="shared" si="73"/>
+        <v>179.58566410388855</v>
+      </c>
+      <c r="I146" t="e">
+        <f t="shared" si="73"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J146">
+        <f t="shared" si="73"/>
+        <v>300.17106749256078</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10">
+      <c r="A147" t="s">
+        <v>13</v>
+      </c>
+      <c r="B147">
+        <f t="shared" ref="B147:J147" si="74">(B114+B125)/$A$84</f>
+        <v>226.81591468176595</v>
+      </c>
+      <c r="C147">
+        <f t="shared" si="74"/>
+        <v>168.27185181123656</v>
+      </c>
+      <c r="D147">
+        <f t="shared" si="74"/>
+        <v>157.58716804202041</v>
+      </c>
+      <c r="E147">
+        <f t="shared" si="74"/>
+        <v>151.14171201575667</v>
+      </c>
+      <c r="F147">
+        <f t="shared" si="74"/>
+        <v>159.06115156031015</v>
+      </c>
+      <c r="G147">
+        <f t="shared" si="74"/>
+        <v>180.0559533291237</v>
+      </c>
+      <c r="H147">
+        <f t="shared" si="74"/>
+        <v>233.26773236452721</v>
+      </c>
+      <c r="I147">
+        <f t="shared" si="74"/>
+        <v>300.17106749256078</v>
+      </c>
+      <c r="J147" t="e">
+        <f t="shared" si="74"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>